<commit_message>
Updated code, README.md file
</commit_message>
<xml_diff>
--- a/src/test/resources/data/SearchData.xlsx
+++ b/src/test/resources/data/SearchData.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EE45157-11CB-45DE-86CA-DE0F0AFA2D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{74E568A9-2C9B-4A3E-BD1B-17B6B4EC0FB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6600" yWindow="4770" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchData" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="63">
   <si>
     <t>testname</t>
   </si>
@@ -63,9 +59,6 @@
     <t>sortByOption</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
     <t>chrome</t>
   </si>
   <si>
@@ -102,9 +95,6 @@
     <t>price</t>
   </si>
   <si>
-    <t>Quick view</t>
-  </si>
-  <si>
     <t>More</t>
   </si>
   <si>
@@ -114,9 +104,6 @@
     <t>Colour</t>
   </si>
   <si>
-    <t>selectProductSort</t>
-  </si>
-  <si>
     <t>left_column</t>
   </si>
   <si>
@@ -162,61 +149,67 @@
     <t>Highest price first</t>
   </si>
   <si>
+    <t>icon-ok</t>
+  </si>
+  <si>
+    <t>fancybox-inner</t>
+  </si>
+  <si>
+    <t>fancybox-item fancybox-close</t>
+  </si>
+  <si>
+    <t>Cas</t>
+  </si>
+  <si>
+    <t>verifySearchedProductsWithProductTypeTest_TC_002</t>
+  </si>
+  <si>
+    <t>verifySearchedProductsWithProductNameTest_TC_001</t>
+  </si>
+  <si>
+    <t>verifyProductElementsAreDisplayedTest_TC_003</t>
+  </si>
+  <si>
+    <t>verifyPopUpIsShownOnClickingProdContainerBtnTest_TC_004</t>
+  </si>
+  <si>
+    <t>verifyProductDescriptionPageIsDisplayedTest_TC_005</t>
+  </si>
+  <si>
+    <t>verifySearchPageFieldIsDisplayedTest_TC_008</t>
+  </si>
+  <si>
+    <t>verifyRequiredSearchPageViewIsSelectedTest_TC_007</t>
+  </si>
+  <si>
+    <t>verifySearchedProductsAreSortedByNameTest_TC_006</t>
+  </si>
+  <si>
+    <t>verifySearchedProductsAreSortedByPriceTest_TC_006</t>
+  </si>
+  <si>
+    <t>verifyAutoSuggestionAndRelatedProductsTest_TC_009</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>uniform-selectProductSort</t>
+  </si>
+  <si>
     <t>Add to cart</t>
   </si>
   <si>
     <t>Add to Wishlist</t>
   </si>
   <si>
-    <t>icon-ok</t>
-  </si>
-  <si>
-    <t>fancybox-inner</t>
-  </si>
-  <si>
-    <t>fancybox-item fancybox-close</t>
-  </si>
-  <si>
-    <t>Cas</t>
-  </si>
-  <si>
-    <t>verifySearchedProductsWithProductTypeTest_TC_002</t>
-  </si>
-  <si>
-    <t>verifySearchedProductsWithProductNameTest_TC_001</t>
-  </si>
-  <si>
-    <t>verifyProductElementsAreDisplayedTest_TC_003</t>
-  </si>
-  <si>
-    <t>verifyPopUpIsShownOnClickingProdContainerBtnTest_TC_004</t>
-  </si>
-  <si>
-    <t>verifyProductDescriptionPageIsDisplayedTest_TC_005</t>
-  </si>
-  <si>
-    <t>verifySearchPageFieldIsDisplayedTest_TC_008</t>
-  </si>
-  <si>
-    <t>verifyRequiredSearchPageViewIsSelectedTest_TC_007</t>
-  </si>
-  <si>
-    <t>verifySearchedProductsAreSortedByNameTest_TC_006</t>
-  </si>
-  <si>
-    <t>verifySearchedProductsAreSortedByPriceTest_TC_006</t>
-  </si>
-  <si>
-    <t>verifyAutoSuggestionAndRelatedProductsTest_TC_009</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t/>
+    <t>Quick</t>
   </si>
 </sst>
 </file>
@@ -538,8 +531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,7 +542,7 @@
     <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="44.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="28.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="45.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="14.140625" bestFit="1" customWidth="1"/>
@@ -596,838 +589,838 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>